<commit_message>
Added a solid faraday cage design and updated BOM
</commit_message>
<xml_diff>
--- a/SolidworksFiles/BOM.xlsx
+++ b/SolidworksFiles/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\code\RSA\RSA-Substation-Inspection-Robot\SolidworksFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09731C6C-17DE-44B8-8610-03CAE5F6FE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5400A208-1DC4-47FA-B78D-7CD0A1750C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5460" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOP Level" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -153,6 +153,42 @@
   </si>
   <si>
     <t>Reference model for a terminal block socket 3-way https://nl.farnell.com/phoenix-contact/1843619/connector-header-tht-3-5mm-3way/dp/3704828?MER=sy-me-pd-mi-acce</t>
+  </si>
+  <si>
+    <t>M-Rivet-Nut</t>
+  </si>
+  <si>
+    <t>Reference model for M4 rivet nut: https://uk.farnell.com/tr-fastenings/w-m4-rede-oe-st-kg/rivet-nut-steel-electro-zinc-cr3/dp/2983977</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>M-RP-CAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part </t>
+  </si>
+  <si>
+    <t>Reference model for Raspberry Pi Camera Module 3: https://datasheets.raspberrypi.com/camera/camera-module-3-standard-mechanical-drawing.pdf</t>
+  </si>
+  <si>
+    <t>M-SmartDriveDuo-10</t>
+  </si>
+  <si>
+    <t>Reference model for SmartDriveDuo-10: https://docs.google.com/document/d/1ECKsH1WfgZLomwFoPQ8PlkUzVEm88A6Sup9X0wDBHKA/view</t>
+  </si>
+  <si>
+    <t>M-TL-FC111B-20</t>
+  </si>
+  <si>
+    <t>Reference model for TL-FC111B-20: https://www.tp-link.com/nl/business-networking/accessory/tl-fc111b-20/</t>
+  </si>
+  <si>
+    <t>M-12V-12Ah-Lead-Acid</t>
+  </si>
+  <si>
+    <t>Reference model for Multipower 12V 12Ah lead acid (4.8mm): https://eu.nkon.nl/rechargeable/lead-acid-batteries/12v-vrla/multipower-12v-12ah-48.html</t>
   </si>
 </sst>
 </file>
@@ -597,19 +633,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884B3ED9-A619-4A4D-95F9-8E1D3298BEF1}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="136.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="158.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +656,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -631,7 +667,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -642,7 +678,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -653,7 +689,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -664,7 +700,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -675,7 +711,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -686,7 +722,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -697,7 +733,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -706,6 +742,76 @@
       </c>
       <c r="C9" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start of electronic box design
</commit_message>
<xml_diff>
--- a/SolidworksFiles/BOM.xlsx
+++ b/SolidworksFiles/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\code\RSA\RSA-Substation-Inspection-Robot\SolidworksFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5400A208-1DC4-47FA-B78D-7CD0A1750C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4284A6EF-EFF5-4F78-AEFB-693832224DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1635" yWindow="2625" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOP Level" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -636,13 +636,13 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="158.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -754,9 +754,6 @@
       <c r="C10" t="s">
         <v>43</v>
       </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -796,9 +793,6 @@
       <c r="C13" t="s">
         <v>51</v>
       </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -809,9 +803,6 @@
       </c>
       <c r="C14" t="s">
         <v>53</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created the Electronic Box cut outs
</commit_message>
<xml_diff>
--- a/SolidworksFiles/BOM.xlsx
+++ b/SolidworksFiles/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\code\RSA\RSA-Substation-Inspection-Robot\SolidworksFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4284A6EF-EFF5-4F78-AEFB-693832224DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7546BA8F-761B-415D-9D1A-08E3F3ADFD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1635" yWindow="2625" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOP Level" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
   <si>
     <t>ID</t>
   </si>
@@ -189,6 +189,30 @@
   </si>
   <si>
     <t>Reference model for Multipower 12V 12Ah lead acid (4.8mm): https://eu.nkon.nl/rechargeable/lead-acid-batteries/12v-vrla/multipower-12v-12ah-48.html</t>
+  </si>
+  <si>
+    <t>M-12V-1A-Lead-Battery-Charger</t>
+  </si>
+  <si>
+    <t>https://nl.rs-online.com/web/p/battery-chargers/4784077</t>
+  </si>
+  <si>
+    <t>M-12V-Connector</t>
+  </si>
+  <si>
+    <t>size reference: https://nl.rs-online.com/web/p/dc-power-connectors/8787203</t>
+  </si>
+  <si>
+    <t>M-Emergency-Switch</t>
+  </si>
+  <si>
+    <t>https://www.conrad.nl/nl/p/tru-components-las1-by-11tsb-noodstopschakelaar-250-v-ac-3-a-1x-nc-1x-no-ip40-1-stuk-s-704766.html?refresh=true#productTechData</t>
+  </si>
+  <si>
+    <t>M-On-Off-Switch</t>
+  </si>
+  <si>
+    <t>https://www.conrad.nl/nl/p/arcolectric-bulgin-ltd-c6053alnah-wipschakelaar-c6053alnah-230-v-ac-16-a-2x-uit-aan-continu-1-stuk-s-701528.html</t>
   </si>
 </sst>
 </file>
@@ -633,15 +657,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884B3ED9-A619-4A4D-95F9-8E1D3298BEF1}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -803,6 +827,50 @@
       </c>
       <c r="C14" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All files 3d print ready
</commit_message>
<xml_diff>
--- a/SolidworksFiles/BOM.xlsx
+++ b/SolidworksFiles/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joona\Documents\GitHub\RSA-Substation-Inspection-Robot\SolidworksFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F9F61-B45E-479C-95BA-23156E82B9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5700E4F8-E618-4960-9C72-C4327D4C9C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -757,7 +757,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added 4 endcap2 prints
</commit_message>
<xml_diff>
--- a/SolidworksFiles/BOM.xlsx
+++ b/SolidworksFiles/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joona\Documents\GitHub\RSA-Substation-Inspection-Robot\SolidworksFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\code\RSA\RSA-Substation-Inspection-Robot\SolidworksFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7AF7A8-7976-4C53-BAD2-0AFABEC65A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D58F16-6A88-418C-A912-97C721B1BA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOP Level" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="95">
   <si>
     <t>ID</t>
   </si>
@@ -310,6 +321,9 @@
   </si>
   <si>
     <t>Half should be mirrored</t>
+  </si>
+  <si>
+    <t>Jeroen</t>
   </si>
 </sst>
 </file>
@@ -757,7 +771,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,6 +888,12 @@
       <c r="D6">
         <v>8</v>
       </c>
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -933,7 +953,7 @@
       </c>
       <c r="F10">
         <f>SUM(F2:F9)</f>
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>